<commit_message>
plotted probability vs age
</commit_message>
<xml_diff>
--- a/data/Aircraft.xlsx
+++ b/data/Aircraft.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyas/Desktop/Workspace/FastStream Tech/Engine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyas/Desktop/Workspace/FastStream Tech/Engine/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="53">
   <si>
     <t>Engine</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>normal</t>
+  </si>
+  <si>
+    <t>n1_age</t>
+  </si>
+  <si>
+    <t>n2_age</t>
   </si>
 </sst>
 </file>
@@ -56834,10 +56840,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -56852,7 +56858,7 @@
     <col min="8" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -56871,26 +56877,32 @@
       <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -56900,9 +56912,9 @@
       <c r="F2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -56921,26 +56933,26 @@
       <c r="F3" s="5">
         <v>12000</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -56959,26 +56971,26 @@
       <c r="F4" s="5">
         <v>11000</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -56997,14 +57009,8 @@
       <c r="F5" s="9">
         <v>7000</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>46</v>
@@ -57013,10 +57019,16 @@
         <v>47</v>
       </c>
       <c r="L5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="N5" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="5">
         <v>1</v>
       </c>
@@ -57035,26 +57047,26 @@
       <c r="F6" s="5">
         <v>10000</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="N6" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -57073,26 +57085,26 @@
       <c r="F7" s="5">
         <v>11000</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="J7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="M7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -57111,26 +57123,26 @@
       <c r="F8" s="9">
         <v>6800</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="K8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="L8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="M8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="N8" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
         <v>2</v>
       </c>
@@ -57149,26 +57161,26 @@
       <c r="F9" s="9">
         <v>7000</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="I9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="J9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="K9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="M9" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="N9" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
         <v>2</v>
       </c>
@@ -57187,26 +57199,26 @@
       <c r="F10" s="5">
         <v>10500</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="J10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="K10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="M10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="N10" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11" s="7">
         <v>2</v>
       </c>
@@ -57225,26 +57237,26 @@
       <c r="F11" s="5">
         <v>10000</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="J11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="K11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="M11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="N11" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
         <v>2</v>
       </c>
@@ -57263,26 +57275,26 @@
       <c r="F12" s="9">
         <v>5000</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="I12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="J12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="K12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="M12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="N12" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16" s="5">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
generating normal data complete
</commit_message>
<xml_diff>
--- a/data/Aircraft.xlsx
+++ b/data/Aircraft.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-27320" yWindow="440" windowWidth="27320" windowHeight="14920" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-27320" yWindow="440" windowWidth="27320" windowHeight="14920" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="final" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="64">
   <si>
     <t>Engine</t>
   </si>
@@ -57413,8 +57414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView topLeftCell="D1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -58872,4 +58873,111 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="7">
+        <v>700</v>
+      </c>
+      <c r="B2" s="5">
+        <v>4500</v>
+      </c>
+      <c r="C2" s="5">
+        <v>10000</v>
+      </c>
+      <c r="D2" s="5">
+        <v>11500</v>
+      </c>
+      <c r="E2" s="5">
+        <v>120</v>
+      </c>
+      <c r="F2" s="5">
+        <v>35</v>
+      </c>
+      <c r="G2" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="7">
+        <v>1750</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5350</v>
+      </c>
+      <c r="C3" s="5">
+        <v>13500</v>
+      </c>
+      <c r="D3" s="5">
+        <v>8000</v>
+      </c>
+      <c r="E3" s="5">
+        <v>137</v>
+      </c>
+      <c r="F3" s="5">
+        <v>-35</v>
+      </c>
+      <c r="G3" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="7">
+        <v>1300</v>
+      </c>
+      <c r="B4" s="7">
+        <v>5000</v>
+      </c>
+      <c r="C4" s="7">
+        <v>12000</v>
+      </c>
+      <c r="D4" s="7">
+        <v>10000</v>
+      </c>
+      <c r="E4" s="7">
+        <v>130</v>
+      </c>
+      <c r="F4" s="7">
+        <v>-10</v>
+      </c>
+      <c r="G4" s="7">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
generated new data but prediction didn't get better
</commit_message>
<xml_diff>
--- a/data/Aircraft.xlsx
+++ b/data/Aircraft.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-27320" yWindow="440" windowWidth="27320" windowHeight="14920" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="final" sheetId="5" r:id="rId5"/>
+    <sheet name="output" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="77">
   <si>
     <t>Engine</t>
   </si>
@@ -221,6 +222,45 @@
   <si>
     <t>air_Temp</t>
   </si>
+  <si>
+    <t>Fuel Filter</t>
+  </si>
+  <si>
+    <t>Low Pressure Fan (N1)</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Fan Blade</t>
+  </si>
+  <si>
+    <t>High Pressure Fan (N2)</t>
+  </si>
+  <si>
+    <t>Actual Life Span (in months)</t>
+  </si>
+  <si>
+    <t>Predicted Life Span (in months)</t>
+  </si>
+  <si>
+    <t>Total Turbine</t>
+  </si>
+  <si>
+    <t>Under normal conditions, Fan Blade starts to deteriorate during month 40 and will last a total of 58 months. But, the Fan Blade deteriorated during month 13 and will last only till month 54.</t>
+  </si>
+  <si>
+    <t>EGT</t>
+  </si>
+  <si>
+    <t>Under normal conditions, EGT starts to exceed limits during month 41 and will last a total of 58 months. But, it exceeded the limits during month 12 and will last only till month 54.</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
 </sst>
 </file>
 
@@ -298,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -331,6 +371,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -58877,10 +58923,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -58977,6 +59023,221 @@
         <v>50</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="7">
+        <v>700</v>
+      </c>
+      <c r="B10" s="5">
+        <v>4500</v>
+      </c>
+      <c r="C10" s="5">
+        <v>10000</v>
+      </c>
+      <c r="D10" s="5">
+        <v>12000</v>
+      </c>
+      <c r="E10" s="5">
+        <v>120</v>
+      </c>
+      <c r="F10" s="5">
+        <v>35</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="7">
+        <v>1900</v>
+      </c>
+      <c r="B11" s="5">
+        <v>5500</v>
+      </c>
+      <c r="C11" s="5">
+        <v>14000</v>
+      </c>
+      <c r="D11" s="5">
+        <v>8000</v>
+      </c>
+      <c r="E11" s="5">
+        <v>137</v>
+      </c>
+      <c r="F11" s="5">
+        <v>-35</v>
+      </c>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="7">
+        <v>1300</v>
+      </c>
+      <c r="B12" s="7">
+        <v>5000</v>
+      </c>
+      <c r="C12" s="7">
+        <v>12000</v>
+      </c>
+      <c r="D12" s="7">
+        <v>10000</v>
+      </c>
+      <c r="E12" s="7">
+        <v>130</v>
+      </c>
+      <c r="F12" s="7">
+        <v>-10</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="20" style="12" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="61.6640625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="12"/>
+    <col min="7" max="8" width="10.83203125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="12"/>
+    <col min="10" max="11" width="10.83203125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="12"/>
+    <col min="13" max="14" width="10.83203125" style="12" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="12">
+        <v>58</v>
+      </c>
+      <c r="C3" s="12">
+        <v>54</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="13"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="12">
+        <v>58</v>
+      </c>
+      <c r="C5" s="12">
+        <v>51</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="13"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="12">
+        <v>60</v>
+      </c>
+      <c r="C7" s="12">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" s="13"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="12">
+        <v>59</v>
+      </c>
+      <c r="C9" s="12">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="13"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="12">
+        <v>58</v>
+      </c>
+      <c r="C11" s="12">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="12">
+        <v>60</v>
+      </c>
+      <c r="C13" s="12">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
very close to final output
</commit_message>
<xml_diff>
--- a/data/Aircraft.xlsx
+++ b/data/Aircraft.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-27320" yWindow="440" windowWidth="27320" windowHeight="14920" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="78">
   <si>
     <t>Engine</t>
   </si>
@@ -229,9 +229,6 @@
     <t>Low Pressure Fan (N1)</t>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>Component</t>
   </si>
   <si>
@@ -250,16 +247,22 @@
     <t>Total Turbine</t>
   </si>
   <si>
-    <t>Under normal conditions, Fan Blade starts to deteriorate during month 40 and will last a total of 58 months. But, the Fan Blade deteriorated during month 13 and will last only till month 54.</t>
-  </si>
-  <si>
     <t>EGT</t>
   </si>
   <si>
-    <t>Under normal conditions, EGT starts to exceed limits during month 41 and will last a total of 58 months. But, it exceeded the limits during month 12 and will last only till month 54.</t>
+    <t>new</t>
   </si>
   <si>
-    <t>new</t>
+    <t>Start month of failure</t>
+  </si>
+  <si>
+    <t>Value of complete failure</t>
+  </si>
+  <si>
+    <t>Value when failure started</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -58923,34 +58926,37 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="7"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
         <v>62</v>
       </c>
     </row>
@@ -59024,92 +59030,87 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>76</v>
+      <c r="A7" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
+      <c r="A9" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F9" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="7">
-        <v>700</v>
-      </c>
-      <c r="B10" s="5">
-        <v>4500</v>
-      </c>
-      <c r="C10" s="5">
-        <v>10000</v>
-      </c>
-      <c r="D10" s="5">
-        <v>12000</v>
-      </c>
-      <c r="E10" s="5">
-        <v>120</v>
-      </c>
-      <c r="F10" s="5">
-        <v>35</v>
-      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="7">
-        <v>1900</v>
-      </c>
-      <c r="B11" s="5">
-        <v>5500</v>
-      </c>
-      <c r="C11" s="5">
-        <v>14000</v>
-      </c>
-      <c r="D11" s="5">
-        <v>8000</v>
-      </c>
-      <c r="E11" s="5">
-        <v>137</v>
-      </c>
-      <c r="F11" s="5">
-        <v>-35</v>
-      </c>
+        <v>1300</v>
+      </c>
+      <c r="B11" s="7">
+        <v>5000</v>
+      </c>
+      <c r="C11" s="7">
+        <v>12000</v>
+      </c>
+      <c r="D11" s="7">
+        <v>10000</v>
+      </c>
+      <c r="E11" s="7">
+        <v>130</v>
+      </c>
+      <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
-        <v>1300</v>
-      </c>
-      <c r="B12" s="7">
-        <v>5000</v>
-      </c>
-      <c r="C12" s="7">
+        <v>1900</v>
+      </c>
+      <c r="B12" s="5">
+        <v>5500</v>
+      </c>
+      <c r="C12" s="5">
+        <v>14000</v>
+      </c>
+      <c r="D12" s="7">
         <v>12000</v>
       </c>
-      <c r="D12" s="7">
-        <v>10000</v>
-      </c>
-      <c r="E12" s="7">
-        <v>130</v>
-      </c>
-      <c r="F12" s="7">
-        <v>-10</v>
-      </c>
-      <c r="G12" s="7"/>
+      <c r="E12" s="5">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="7">
+        <v>2500</v>
+      </c>
+      <c r="B13" s="7">
+        <v>6000</v>
+      </c>
+      <c r="C13" s="7">
+        <v>16000</v>
+      </c>
+      <c r="D13" s="7">
+        <v>14000</v>
+      </c>
+      <c r="E13" s="7">
+        <v>143</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -59118,77 +59119,87 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="121" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20" style="12" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="61.6640625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="12"/>
-    <col min="7" max="8" width="10.83203125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="12"/>
+    <col min="1" max="1" width="20" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="10.83203125" style="12" customWidth="1"/>
     <col min="12" max="12" width="10.83203125" style="12"/>
     <col min="13" max="14" width="10.83203125" style="12" customWidth="1"/>
     <col min="15" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="13" t="s">
-        <v>68</v>
-      </c>
       <c r="B3" s="12">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C3" s="12">
-        <v>54</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+        <v>143.11000000000001</v>
+      </c>
+      <c r="D3" s="12">
+        <v>32</v>
+      </c>
+      <c r="E3" s="12">
+        <v>137.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="13"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="12">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C5" s="12">
-        <v>51</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+        <v>2468</v>
+      </c>
+      <c r="D5" s="12">
+        <v>32</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="13"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
         <v>64</v>
       </c>
@@ -59196,13 +59207,19 @@
         <v>60</v>
       </c>
       <c r="C7" s="12">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+        <v>5968</v>
+      </c>
+      <c r="D7" s="12">
+        <v>32</v>
+      </c>
+      <c r="E7" s="12">
+        <v>5504</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="13"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="13" t="s">
         <v>65</v>
       </c>
@@ -59210,32 +59227,181 @@
         <v>59</v>
       </c>
       <c r="C9" s="12">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+        <v>15914</v>
+      </c>
+      <c r="D9" s="12">
+        <v>31</v>
+      </c>
+      <c r="E9" s="12">
+        <v>14003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="13"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="12">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C11" s="12">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+        <v>13935</v>
+      </c>
+      <c r="D11" s="12">
+        <v>32</v>
+      </c>
+      <c r="E11" s="12">
+        <v>12068</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="12">
         <v>60</v>
       </c>
-      <c r="C13" s="12">
-        <v>53</v>
+      <c r="C13" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="12">
+        <v>31</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="12">
+        <v>31</v>
+      </c>
+      <c r="C20" s="12">
+        <v>144.9</v>
+      </c>
+      <c r="D20" s="12">
+        <v>14</v>
+      </c>
+      <c r="E20" s="12">
+        <v>136.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="13"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="12">
+        <v>30</v>
+      </c>
+      <c r="C22" s="12">
+        <v>2528</v>
+      </c>
+      <c r="D22" s="12">
+        <v>16</v>
+      </c>
+      <c r="E22" s="12">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" s="13"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="12">
+        <v>38</v>
+      </c>
+      <c r="C24" s="12">
+        <v>6442</v>
+      </c>
+      <c r="D24" s="12">
+        <v>14</v>
+      </c>
+      <c r="E24" s="12">
+        <v>5511</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" s="13"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="12">
+        <v>36</v>
+      </c>
+      <c r="C26" s="12">
+        <v>15557</v>
+      </c>
+      <c r="D26" s="12">
+        <v>21</v>
+      </c>
+      <c r="E26" s="12">
+        <v>13939</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" s="13"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="12">
+        <v>36</v>
+      </c>
+      <c r="C28" s="12">
+        <v>13617</v>
+      </c>
+      <c r="D28" s="12">
+        <v>21</v>
+      </c>
+      <c r="E28" s="12">
+        <v>11967</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="12">
+        <v>36</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="12">
+        <v>15</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>